<commit_message>
worked on Motor SVM
</commit_message>
<xml_diff>
--- a/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/PythonClassifierApplication_Getr/Ergebnisse_linSVM_Getriebe_C.xlsx
+++ b/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/PythonClassifierApplication_Getr/Ergebnisse_linSVM_Getriebe_C.xlsx
@@ -451,7 +451,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +645,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F11" s="10">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G11" s="2">
         <v>0.87227290000000002</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F12" s="10">
-        <v>9.9999999999999995E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="G12" s="2">
         <v>0.83352630000000005</v>

</xml_diff>

<commit_message>
updated excel files containing classification metrics
</commit_message>
<xml_diff>
--- a/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/PythonClassifierApplication_Getr/Ergebnisse_linSVM_Getriebe_C.xlsx
+++ b/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/PythonClassifierApplication_Getr/Ergebnisse_linSVM_Getriebe_C.xlsx
@@ -41,13 +41,13 @@
     <t>(auf 7 Stellen gerundet)</t>
   </si>
   <si>
-    <t>Mean Accuracy</t>
-  </si>
-  <si>
     <t>C-Parameter</t>
   </si>
   <si>
     <t>lineare SVM</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,10 +466,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>0</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="11">
         <v>100000</v>

</xml_diff>